<commit_message>
Excel Plotter, Updated Qidi Prts
Excel Plotter, Updated Qidi Prts
</commit_message>
<xml_diff>
--- a/Firmware_Examples/Euclid_Macro_Path_Plot.xlsx
+++ b/Firmware_Examples/Euclid_Macro_Path_Plot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\Euclid_Probe\Firmware_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C22295-1969-41C4-9599-58F37E9584A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495154C6-617B-4FB7-8EA3-6329A9D15F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="167" xr2:uid="{420C2AD8-3186-4775-AC75-27693F26464F}"/>
+    <workbookView xWindow="1920" yWindow="1365" windowWidth="21600" windowHeight="12930" tabRatio="167" xr2:uid="{420C2AD8-3186-4775-AC75-27693F26464F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3F20110-E91B-49C7-9314-26ED469BE75D}" type="CELLRANGE">
+                    <a:fld id="{6BF25F93-70A5-4DF1-A34F-89984640CE66}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -447,7 +447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C61E273-4F6D-42E5-9B41-D187FA89E280}" type="CELLRANGE">
+                    <a:fld id="{5EAEA2DF-026C-4D0A-899E-992E1BD899F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -486,7 +486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0B7C4DD-F78B-404B-8E1E-3EA3E676B9EF}" type="CELLRANGE">
+                    <a:fld id="{613631B9-8003-4BDD-A2EB-5FE8CFCA3FD2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -525,7 +525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{740C9C36-BA04-41F8-ADDF-9AF547CC06BC}" type="CELLRANGE">
+                    <a:fld id="{270CDF55-6D33-474D-88C4-597E892D4A47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -564,7 +564,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF18DF47-F7F9-44AE-9AF2-8DBE8DFC27D1}" type="CELLRANGE">
+                    <a:fld id="{A288657E-1133-4171-93F3-900C96A5F8B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -641,16 +641,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>151</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>175</c:v>
@@ -665,16 +665,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>327</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>327</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>327</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>175</c:v>
@@ -918,7 +918,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>327 347 Z Stop</c:v>
+                  <c:v>235 349 Z Stop</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -961,7 +961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB68A3FB-BFDB-43B6-9827-07741753AD34}" type="CELLRANGE">
+                    <a:fld id="{F5510731-72AE-4C53-BBBF-2524EA5381FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1046,10 +1046,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>327</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>327</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,10 +1061,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>347</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>347</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,10 +1133,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>327</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1148,10 +1148,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>347</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>327</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2323,7 +2323,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2334,7 +2334,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,11 +2400,11 @@
       </c>
       <c r="R4">
         <f>R11</f>
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="S4">
         <f>S12</f>
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="T4" t="s">
         <v>22</v>
@@ -2423,11 +2423,11 @@
       </c>
       <c r="R5">
         <f>C6</f>
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="S5">
         <f>D6</f>
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="T5" t="s">
         <v>14</v>
@@ -2441,10 +2441,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="2">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -2464,12 +2464,12 @@
         <v>350</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:R9" si="0">C7</f>
-        <v>46</v>
+        <f t="shared" ref="R6:R7" si="0">C7</f>
+        <v>35</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6:S9" si="1">D7</f>
-        <v>275</v>
+        <f t="shared" ref="S6:S7" si="1">D7</f>
+        <v>320</v>
       </c>
       <c r="T6" t="s">
         <v>15</v>
@@ -2483,10 +2483,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2">
-        <v>275</v>
+        <v>320</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -2507,11 +2507,11 @@
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="S7">
         <f t="shared" si="1"/>
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -2525,10 +2525,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -2549,11 +2549,11 @@
       </c>
       <c r="R8">
         <f>C12</f>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="S8">
         <f>D12</f>
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="T8" t="s">
         <v>16</v>
@@ -2567,10 +2567,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="D9" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -2636,11 +2636,11 @@
       </c>
       <c r="R11">
         <f>C9</f>
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="S11">
         <f>D9</f>
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="T11" t="s">
         <v>22</v>
@@ -2654,10 +2654,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="2">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D12" s="2">
-        <v>327</v>
+        <v>349</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -2676,11 +2676,11 @@
       </c>
       <c r="R12">
         <f>R11</f>
-        <v>327</v>
+        <v>235</v>
       </c>
       <c r="S12">
         <f>S11</f>
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>